<commit_message>
Updated the maven versions of the jar files. Added generic methods for Automatic booking. Updated excel sheet. Updated the Chrome driver.exe version.
</commit_message>
<xml_diff>
--- a/PageFactory_FrameWork/uiAutomation/src/main/java/com/test/automation/uiAutomation/data/TestData.xlsx
+++ b/PageFactory_FrameWork/uiAutomation/src/main/java/com/test/automation/uiAutomation/data/TestData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13485" windowHeight="6315"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14835" windowHeight="6315" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="automaticBookingTestData" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="70">
   <si>
     <t>email</t>
   </si>
@@ -47,6 +47,186 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>5:00 AM</t>
+  </si>
+  <si>
+    <t>5:15 AM</t>
+  </si>
+  <si>
+    <t>5:30 AM</t>
+  </si>
+  <si>
+    <t>5:45 AM</t>
+  </si>
+  <si>
+    <t>6:00 AM</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>6:15 AM</t>
+  </si>
+  <si>
+    <t>6:30 AM</t>
+  </si>
+  <si>
+    <t>6:45 AM</t>
+  </si>
+  <si>
+    <t>7:00 AM</t>
+  </si>
+  <si>
+    <t>7:15 AM</t>
+  </si>
+  <si>
+    <t>7:30 AM</t>
+  </si>
+  <si>
+    <t>7:45 AM</t>
+  </si>
+  <si>
+    <t>8:00 AM</t>
+  </si>
+  <si>
+    <t>8:15 AM</t>
+  </si>
+  <si>
+    <t>8:30 AM</t>
+  </si>
+  <si>
+    <t>8:45 AM</t>
+  </si>
+  <si>
+    <t>9:00 AM</t>
+  </si>
+  <si>
+    <t>9:15 AM</t>
+  </si>
+  <si>
+    <t>9:30 AM</t>
+  </si>
+  <si>
+    <t>9:45 AM</t>
+  </si>
+  <si>
+    <t>10:00 AM</t>
+  </si>
+  <si>
+    <t>10:15 AM</t>
+  </si>
+  <si>
+    <t>10:30 AM</t>
+  </si>
+  <si>
+    <t>10:45 AM</t>
+  </si>
+  <si>
+    <t>11:00 AM</t>
+  </si>
+  <si>
+    <t>11:15 AM</t>
+  </si>
+  <si>
+    <t>11:30 AM</t>
+  </si>
+  <si>
+    <t>11:45 AM</t>
+  </si>
+  <si>
+    <t>12:00 AM</t>
+  </si>
+  <si>
+    <t>12:15 AM</t>
+  </si>
+  <si>
+    <t>12:30 AM</t>
+  </si>
+  <si>
+    <t>12:45 AM</t>
+  </si>
+  <si>
+    <t>1:00 PM</t>
+  </si>
+  <si>
+    <t>1:15 PM</t>
+  </si>
+  <si>
+    <t>1:30 PM</t>
+  </si>
+  <si>
+    <t>1:45 PM</t>
+  </si>
+  <si>
+    <t>2:00 PM</t>
+  </si>
+  <si>
+    <t>2:15 PM</t>
+  </si>
+  <si>
+    <t>2:30 PM</t>
+  </si>
+  <si>
+    <t>2:45 PM</t>
+  </si>
+  <si>
+    <t>3:00 PM</t>
+  </si>
+  <si>
+    <t>3:15 PM</t>
+  </si>
+  <si>
+    <t>3:30 PM</t>
+  </si>
+  <si>
+    <t>3:45 PM</t>
+  </si>
+  <si>
+    <t>4:00 PM</t>
+  </si>
+  <si>
+    <t>4:15 PM</t>
+  </si>
+  <si>
+    <t>4:30 PM</t>
+  </si>
+  <si>
+    <t>4:45 PM</t>
+  </si>
+  <si>
+    <t>5:00 PM</t>
+  </si>
+  <si>
+    <t>5:15 PM</t>
+  </si>
+  <si>
+    <t>5:30 PM</t>
+  </si>
+  <si>
+    <t>5:45 PM</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -96,9 +276,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,24 +689,1733 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection sqref="A1:E53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" t="s">
+        <v>68</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>